<commit_message>
New table, excel and map ready
</commit_message>
<xml_diff>
--- a/area_tbl.xlsx
+++ b/area_tbl.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">value</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">No protection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
   </si>
   <si>
     <t xml:space="preserve">Production
@@ -413,10 +410,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>351.588884563236</v>
+        <v>2026.65606284671</v>
       </c>
       <c r="C4" t="n">
-        <v>0.814919535887345</v>
+        <v>4.69742273049952</v>
       </c>
     </row>
     <row r="5">
@@ -424,10 +421,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>2026.65606284671</v>
+        <v>736.644195626221</v>
       </c>
       <c r="C5" t="n">
-        <v>4.69742273049952</v>
+        <v>1.70740820421431</v>
       </c>
     </row>
     <row r="6">
@@ -435,21 +432,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>736.644195626221</v>
+        <v>2529.90342608951</v>
       </c>
       <c r="C6" t="n">
-        <v>1.70740820421431</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2178.31454152628</v>
-      </c>
-      <c r="C7" t="n">
-        <v>5.04893969387696</v>
+        <v>5.86385922976431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed table with no next lines
</commit_message>
<xml_diff>
--- a/area_tbl.xlsx
+++ b/area_tbl.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t xml:space="preserve">value</t>
+    <t xml:space="preserve">Protection</t>
   </si>
   <si>
     <t xml:space="preserve">area_km2</t>
@@ -23,24 +23,19 @@
     <t xml:space="preserve">prop_land</t>
   </si>
   <si>
-    <t xml:space="preserve">Insufficient
-legal
-protection</t>
+    <t xml:space="preserve">Insufficient legal protection</t>
   </si>
   <si>
     <t xml:space="preserve">No protection</t>
   </si>
   <si>
-    <t xml:space="preserve">Production
-areas</t>
+    <t xml:space="preserve">Production areas</t>
   </si>
   <si>
     <t xml:space="preserve">Protected areas</t>
   </si>
   <si>
-    <t xml:space="preserve">Requires
-individual
-assessment</t>
+    <t xml:space="preserve">Requires individual assessment</t>
   </si>
 </sst>
 </file>

</xml_diff>